<commit_message>
remove the comment from first method
</commit_message>
<xml_diff>
--- a/testdata/userData.xlsx
+++ b/testdata/userData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhi1\eclipse-workspace\ProjectOn\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10948043-D613-48B8-834F-B4B009AB5770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A873F9-677E-4717-AFA4-F7E27A34F006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{5B4B4FDE-F45B-4E84-AA78-C0C1C1003CF4}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>UserID</t>
   </si>
@@ -446,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E555A34B-5CAF-4B21-B119-FD4EB87647EB}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="A3" sqref="A3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,9 +504,56 @@
         <v>865655446</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>324365</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>873465768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>248999</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>865655446</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{599B5B71-1BFA-4891-A065-BF6088DE364C}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{94F87D2C-DD44-48DC-92DC-659CFFF44E7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>